<commit_message>
se hizo el cambio en la base de datos normalizando estudianteasignatura que venía muy enredado..  se separó en 3 tablas: estudaitneasignatura, ea_grupos y ea_docentes.   y se creó la columna nivel_nota que permite detectar si la defintivia es nula, menos a 3, entre 3 y 3.8 y mayor o igula a 3.8
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807C8322-965C-F34A-8CA2-51FF6093263B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9A57AB-1744-E44E-821C-45720921E7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="680" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="31420" yWindow="500" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>Variables</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>distribución notas previas obtenidas por el estudiante en todas las asignaturas  (%altas, %medias, %bajas)</t>
-  </si>
-  <si>
     <t>2 promedios semestrales previos</t>
   </si>
   <si>
@@ -156,6 +153,15 @@
   </si>
   <si>
     <t>tomó una carga académica inadecuada</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>distribución notas previas obtenidas por el estudiante en todas las asignaturas  (%altas, %medias, %bajas) dos últimos semestres</t>
+  </si>
+  <si>
+    <t>3.2</t>
   </si>
 </sst>
 </file>
@@ -575,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
   <dimension ref="A2:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,7 +602,7 @@
   <sheetData>
     <row r="2" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -607,26 +613,26 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
@@ -634,26 +640,26 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
@@ -662,26 +668,26 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -689,34 +695,34 @@
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="H14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="K14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="L14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -732,8 +738,11 @@
       <c r="A16" s="1">
         <v>1</v>
       </c>
+      <c r="B16" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="C16" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>1</v>
@@ -748,12 +757,15 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:12" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3</v>
       </c>
+      <c r="B17" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="C17" s="6" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
@@ -773,7 +785,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
@@ -793,7 +805,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
@@ -813,7 +825,7 @@
         <v>6.5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -831,7 +843,7 @@
         <v>7.8</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -849,7 +861,7 @@
         <v>9.1</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -867,7 +879,7 @@
         <v>10.4</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -885,7 +897,7 @@
         <v>11.7</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -906,7 +918,7 @@
         <v>13</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
@@ -926,7 +938,7 @@
         <v>14.3</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -942,7 +954,7 @@
         <v>15.6</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -960,7 +972,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -978,7 +990,7 @@
         <v>18.2</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -996,7 +1008,7 @@
         <v>19.5</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -1014,7 +1026,7 @@
         <v>20.8</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1035,7 +1047,7 @@
         <v>22.1</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>

</xml_diff>

<commit_message>
ya se tiene si tuvo acgividades deportivas, culturas u otras en periodos anteriores
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9A57AB-1744-E44E-821C-45720921E7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8BC69D-4D85-EB4F-BDC6-E29B87E01CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31420" yWindow="500" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="17800" yWindow="500" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
   <si>
     <t>Variables</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>3.2</t>
+  </si>
+  <si>
+    <t>3.3</t>
   </si>
 </sst>
 </file>
@@ -209,12 +212,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,15 +264,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
   <dimension ref="A2:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,21 +612,21 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -623,7 +634,7 @@
       <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -631,18 +642,18 @@
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="D6"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
     </row>
@@ -650,7 +661,7 @@
       <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -658,19 +669,18 @@
       <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="11"/>
+      <c r="D9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -678,7 +688,7 @@
       <c r="B11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -686,12 +696,12 @@
       <c r="B12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" s="10"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
@@ -823,6 +833,9 @@
     <row r="20" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>6.5</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
ya calculé la edad que tenía el estudiante cuando tomó el semestre
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8BC69D-4D85-EB4F-BDC6-E29B87E01CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FD846E-325C-DD48-B405-D1DB91F6C104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17800" yWindow="500" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
   <si>
     <t>Variables</t>
   </si>
@@ -165,13 +165,16 @@
   </si>
   <si>
     <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,6 +214,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -238,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -270,10 +281,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -592,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
   <dimension ref="A2:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,15 +629,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
@@ -834,7 +851,7 @@
       <c r="A20" s="1">
         <v>6.5</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -890,6 +907,9 @@
     <row r="23" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>10.4</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>28</v>
@@ -909,6 +929,9 @@
       <c r="A24" s="1">
         <v>11.7</v>
       </c>
+      <c r="B24" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="C24" s="6" t="s">
         <v>29</v>
       </c>
@@ -929,6 +952,9 @@
     <row r="25" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>13</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
para cada d en datos, se obtiene min definitiva en asignturas vistas antes en cada depto.  tambie max, avg y cnt
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FD846E-325C-DD48-B405-D1DB91F6C104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D136EEB-72A2-8745-A88C-BD4D63703559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17800" yWindow="500" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="8580" yWindow="500" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>Variables</t>
   </si>
@@ -168,13 +169,40 @@
   </si>
   <si>
     <t>3.4</t>
+  </si>
+  <si>
+    <t>se mira si al menos fue una vez en el semeste a cursos culturales, deportivos u otros y luego se cuenta cuantas veces lo hizo en pasados semestres</t>
+  </si>
+  <si>
+    <t>se incluyen los resultados por area o si era el total del icfes anterior</t>
+  </si>
+  <si>
+    <t>Para cada semestre se calcula cuantas materias obtuvo sin nota (-1), con nota perdida (1), con nota regular entre 3 y 3.8 (2) o con nota superior o igual a 3.8 (3).  Luego se calcula cuantas veces ocurrió eso en periodos anteriores</t>
+  </si>
+  <si>
+    <t>se calcula la edad que tenía el estudiante al iniciar el semestre</t>
+  </si>
+  <si>
+    <t>Por dpto, min nota obtenida por asignaturas de ese dpto en periodos anteriores</t>
+  </si>
+  <si>
+    <t>Por dpto, max nota obtenida por asignaturas de ese dpto en periodos anteriores</t>
+  </si>
+  <si>
+    <t>Por dpto, avg nota obtenida por asignaturas de ese dpto en periodos anteriores</t>
+  </si>
+  <si>
+    <t>Por dpto, cuantas asig vista  ese dpto en periodos anteriores</t>
+  </si>
+  <si>
+    <t>3.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,19 +250,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -281,17 +318,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,161 +644,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
-  <dimension ref="A2:L88"/>
+  <dimension ref="A2:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="8"/>
-    <col min="3" max="3" width="25.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="25.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="12" t="s">
+    <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D4" s="9"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6"/>
       <c r="F6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D9"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="9"/>
+      <c r="E9"/>
       <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" s="9"/>
-    </row>
-    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="I14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="J14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="K14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="8" t="s">
+      <c r="L14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="D15" s="5"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -771,22 +821,25 @@
       <c r="C16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>1</v>
+      <c r="D16" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" ht="85" x14ac:dyDescent="0.2">
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" ht="105" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>41</v>
@@ -794,192 +847,200 @@
       <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="4"/>
+      <c r="D17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>6.5</v>
-      </c>
-      <c r="B20" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>7.8</v>
+        <v>6</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>9.1</v>
+        <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>10.4</v>
-      </c>
-      <c r="B23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>11.7</v>
-      </c>
-      <c r="B24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K24" s="4"/>
-      <c r="L24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L24" s="4"/>
+      <c r="M24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>13</v>
-      </c>
-      <c r="B25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="4"/>
+      <c r="D25" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="J25" s="4"/>
+      <c r="K25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>14.3</v>
+        <v>11</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -987,108 +1048,102 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>15.6</v>
+        <v>12</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>16.899999999999999</v>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="4"/>
+        <v>48</v>
+      </c>
+      <c r="D28" s="12"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:12" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>18.2</v>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="8" t="s">
+        <v>52</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="D29" s="12"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>19.5</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="12"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>20.8</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D31" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="12"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>22.1</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
@@ -1096,12 +1151,11 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D33" s="4"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1109,19 +1163,33 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D34" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>13</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D35" s="4"/>
+      <c r="K34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>14</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1129,9 +1197,17 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D36" s="4"/>
+      <c r="L35" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>15</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1139,9 +1215,17 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D37" s="4"/>
+      <c r="L36" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>16</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
@@ -1149,9 +1233,20 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D38" s="4"/>
+      <c r="L37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>17</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1159,9 +1254,12 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-    </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -1169,9 +1267,9 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="4"/>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -1179,9 +1277,9 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="4"/>
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -1189,9 +1287,9 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D42" s="4"/>
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -1199,9 +1297,9 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D43" s="4"/>
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1209,9 +1307,9 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D44" s="4"/>
+      <c r="L43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -1219,9 +1317,9 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D45" s="4"/>
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -1229,9 +1327,9 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
-    </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D46" s="4"/>
+      <c r="L45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1239,9 +1337,9 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-    </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D47" s="4"/>
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1249,9 +1347,9 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-    </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D48" s="4"/>
+      <c r="L47" s="4"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -1259,9 +1357,9 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-    </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D49" s="4"/>
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1269,9 +1367,9 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D50" s="4"/>
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
@@ -1279,9 +1377,9 @@
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
-    </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D51" s="4"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1289,9 +1387,9 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
-    </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D52" s="4"/>
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
@@ -1299,9 +1397,9 @@
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D53" s="4"/>
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
@@ -1309,9 +1407,9 @@
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D54" s="4"/>
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -1319,9 +1417,9 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-    </row>
-    <row r="55" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D55" s="4"/>
+      <c r="L54" s="4"/>
+    </row>
+    <row r="55" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -1329,9 +1427,9 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D56" s="4"/>
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -1339,9 +1437,9 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D57" s="4"/>
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
@@ -1349,9 +1447,9 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
-    </row>
-    <row r="58" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D58" s="4"/>
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
@@ -1359,9 +1457,9 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-    </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D59" s="4"/>
+      <c r="L58" s="4"/>
+    </row>
+    <row r="59" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -1369,9 +1467,9 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
-    </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D60" s="4"/>
+      <c r="L59" s="4"/>
+    </row>
+    <row r="60" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -1379,9 +1477,9 @@
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
-    </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D61" s="4"/>
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -1389,9 +1487,9 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
-    </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D62" s="4"/>
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -1399,9 +1497,9 @@
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-    </row>
-    <row r="63" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D63" s="4"/>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -1409,9 +1507,9 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
-    </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D64" s="4"/>
+      <c r="L63" s="4"/>
+    </row>
+    <row r="64" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -1419,9 +1517,9 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-    </row>
-    <row r="65" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D65" s="4"/>
+      <c r="L64" s="4"/>
+    </row>
+    <row r="65" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -1429,9 +1527,9 @@
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
-    </row>
-    <row r="66" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D66" s="4"/>
+      <c r="L65" s="4"/>
+    </row>
+    <row r="66" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -1439,9 +1537,9 @@
       <c r="I66" s="4"/>
       <c r="J66" s="4"/>
       <c r="K66" s="4"/>
-    </row>
-    <row r="67" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D67" s="4"/>
+      <c r="L66" s="4"/>
+    </row>
+    <row r="67" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -1449,9 +1547,9 @@
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
-    </row>
-    <row r="68" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D68" s="4"/>
+      <c r="L67" s="4"/>
+    </row>
+    <row r="68" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -1459,9 +1557,9 @@
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="4"/>
-    </row>
-    <row r="69" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D69" s="4"/>
+      <c r="L68" s="4"/>
+    </row>
+    <row r="69" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -1469,9 +1567,9 @@
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
-    </row>
-    <row r="70" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D70" s="4"/>
+      <c r="L69" s="4"/>
+    </row>
+    <row r="70" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -1479,9 +1577,9 @@
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
-    </row>
-    <row r="71" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D71" s="4"/>
+      <c r="L70" s="4"/>
+    </row>
+    <row r="71" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -1489,9 +1587,9 @@
       <c r="I71" s="4"/>
       <c r="J71" s="4"/>
       <c r="K71" s="4"/>
-    </row>
-    <row r="72" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D72" s="4"/>
+      <c r="L71" s="4"/>
+    </row>
+    <row r="72" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
@@ -1499,9 +1597,9 @@
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
       <c r="K72" s="4"/>
-    </row>
-    <row r="73" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D73" s="4"/>
+      <c r="L72" s="4"/>
+    </row>
+    <row r="73" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
@@ -1509,9 +1607,9 @@
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
       <c r="K73" s="4"/>
-    </row>
-    <row r="74" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D74" s="4"/>
+      <c r="L73" s="4"/>
+    </row>
+    <row r="74" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -1519,9 +1617,9 @@
       <c r="I74" s="4"/>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
-    </row>
-    <row r="75" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D75" s="4"/>
+      <c r="L74" s="4"/>
+    </row>
+    <row r="75" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
@@ -1529,9 +1627,9 @@
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="4"/>
-    </row>
-    <row r="76" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D76" s="4"/>
+      <c r="L75" s="4"/>
+    </row>
+    <row r="76" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -1539,9 +1637,9 @@
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
       <c r="K76" s="4"/>
-    </row>
-    <row r="77" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D77" s="4"/>
+      <c r="L76" s="4"/>
+    </row>
+    <row r="77" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
@@ -1549,9 +1647,9 @@
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
-    </row>
-    <row r="78" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D78" s="4"/>
+      <c r="L77" s="4"/>
+    </row>
+    <row r="78" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -1559,9 +1657,9 @@
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
       <c r="K78" s="4"/>
-    </row>
-    <row r="79" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D79" s="4"/>
+      <c r="L78" s="4"/>
+    </row>
+    <row r="79" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
@@ -1569,9 +1667,9 @@
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
-    </row>
-    <row r="80" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D80" s="4"/>
+      <c r="L79" s="4"/>
+    </row>
+    <row r="80" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
@@ -1579,9 +1677,9 @@
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
       <c r="K80" s="4"/>
-    </row>
-    <row r="81" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D81" s="4"/>
+      <c r="L80" s="4"/>
+    </row>
+    <row r="81" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
@@ -1589,9 +1687,9 @@
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
       <c r="K81" s="4"/>
-    </row>
-    <row r="82" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D82" s="4"/>
+      <c r="L81" s="4"/>
+    </row>
+    <row r="82" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -1599,9 +1697,9 @@
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
-    </row>
-    <row r="83" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D83" s="4"/>
+      <c r="L82" s="4"/>
+    </row>
+    <row r="83" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
@@ -1609,9 +1707,9 @@
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
-    </row>
-    <row r="84" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D84" s="4"/>
+      <c r="L83" s="4"/>
+    </row>
+    <row r="84" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
@@ -1619,9 +1717,9 @@
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
-    </row>
-    <row r="85" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D85" s="4"/>
+      <c r="L84" s="4"/>
+    </row>
+    <row r="85" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
@@ -1629,9 +1727,9 @@
       <c r="I85" s="4"/>
       <c r="J85" s="4"/>
       <c r="K85" s="4"/>
-    </row>
-    <row r="86" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D86" s="4"/>
+      <c r="L85" s="4"/>
+    </row>
+    <row r="86" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
@@ -1639,9 +1737,9 @@
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
       <c r="K86" s="4"/>
-    </row>
-    <row r="87" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D87" s="4"/>
+      <c r="L86" s="4"/>
+    </row>
+    <row r="87" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
@@ -1649,9 +1747,9 @@
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
       <c r="K87" s="4"/>
-    </row>
-    <row r="88" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D88" s="4"/>
+      <c r="L87" s="4"/>
+    </row>
+    <row r="88" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
@@ -1659,10 +1757,71 @@
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
       <c r="K88" s="4"/>
+      <c r="L88" s="4"/>
+    </row>
+    <row r="89" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E89" s="4"/>
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+    </row>
+    <row r="90" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+    </row>
+    <row r="91" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+    </row>
+    <row r="92" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+    </row>
+    <row r="93" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="4"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+    </row>
+    <row r="94" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="4"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ya se calula la experiencia docente promedio de los docentes de las asiganturas por departamento, que tenian en periodos anteriores a cuando el estudiante tomó la asignatura en el periodo p.  mirar 3.6
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D136EEB-72A2-8745-A88C-BD4D63703559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F4C0B4-6DF6-2547-8CA9-4ED9F1A8BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="500" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="20800" yWindow="5040" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
   <si>
     <t>Variables</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Demografia docente:  distribución por genero</t>
   </si>
   <si>
-    <t>Experiencia docente promedio utlimos 2 semestres</t>
-  </si>
-  <si>
     <t>promedio tamaño cursos que ha tomado ultimos 2 semestres</t>
   </si>
   <si>
@@ -196,6 +193,12 @@
   </si>
   <si>
     <t>3.5</t>
+  </si>
+  <si>
+    <t>Experiencia docente promedio por dpto (min, max, avg)</t>
+  </si>
+  <si>
+    <t>3.6</t>
   </si>
 </sst>
 </file>
@@ -266,12 +269,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -286,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -329,6 +338,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
   <dimension ref="A2:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,10 +769,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="D12" s="9"/>
     </row>
@@ -798,7 +810,7 @@
         <v>20</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -816,13 +828,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>1</v>
@@ -842,13 +854,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
@@ -908,13 +920,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -968,7 +980,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>28</v>
@@ -989,7 +1001,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>29</v>
@@ -1013,13 +1025,13 @@
         <v>10</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
@@ -1072,10 +1084,10 @@
     <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="4"/>
@@ -1090,10 +1102,10 @@
     <row r="29" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="4"/>
@@ -1108,10 +1120,10 @@
     <row r="30" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="4"/>
@@ -1126,10 +1138,10 @@
     <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="4"/>
@@ -1141,8 +1153,14 @@
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
+      <c r="B32" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="D32" s="12"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1165,12 +1183,9 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
     </row>
-    <row r="34" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>13</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1188,7 +1203,7 @@
         <v>14</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1224,7 +1239,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1245,7 +1260,7 @@
         <v>17</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>

</xml_diff>

<commit_message>
ya calcula los promedios semestrales hace 1, 2, .. semestres
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F4C0B4-6DF6-2547-8CA9-4ED9F1A8BA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C275A0B0-2AB8-4D4E-BF49-3EE9470B1680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20800" yWindow="5040" windowWidth="33400" windowHeight="24080" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
+    <workbookView xWindow="27520" yWindow="2800" windowWidth="23120" windowHeight="23040" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
   <si>
     <t>Variables</t>
   </si>
@@ -195,10 +194,43 @@
     <t>3.5</t>
   </si>
   <si>
-    <t>Experiencia docente promedio por dpto (min, max, avg)</t>
-  </si>
-  <si>
     <t>3.6</t>
+  </si>
+  <si>
+    <t>Experiencia docente cursos previos promedio por dpto (min, max, avg, stddev)</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>Experiencia docente cursos que va a ver en el periodo actual promedio por dpto (min, max, avg, stddev)</t>
+  </si>
+  <si>
+    <t>FECHA 1</t>
+  </si>
+  <si>
+    <t>9 DE DICIEMBRE</t>
+  </si>
+  <si>
+    <t>FECHA 2</t>
+  </si>
+  <si>
+    <t>22 DE ENERO</t>
+  </si>
+  <si>
+    <t>VIDEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ya usar un powerpoint de cómo voy </t>
+  </si>
+  <si>
+    <t>dedicarse solo al tema de procesamiento, modelos</t>
+  </si>
+  <si>
+    <t>no el sustento del problema etc….</t>
+  </si>
+  <si>
+    <t>FECHA:  3 DE NOVIEMBRE</t>
   </si>
 </sst>
 </file>
@@ -269,18 +301,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -295,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,13 +359,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -658,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
   <dimension ref="A2:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,16 +707,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
@@ -1122,7 +1151,7 @@
       <c r="B30" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>49</v>
       </c>
       <c r="D30" s="12"/>
@@ -1140,7 +1169,7 @@
       <c r="B31" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D31" s="12"/>
@@ -1155,11 +1184,11 @@
     </row>
     <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="4"/>
@@ -1168,11 +1197,19 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
+      <c r="K32" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L32" s="4"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
+      <c r="B33" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="D33" s="12"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -1294,7 +1331,13 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B41" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -1304,7 +1347,13 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B42" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -1334,7 +1383,13 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B45" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -1344,7 +1399,10 @@
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="C46" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1354,7 +1412,10 @@
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="C47" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1364,7 +1425,10 @@
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="C48" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>

</xml_diff>

<commit_message>
ya se cargóla historia del tamaño de los grupos y al cosa mejoró
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C275A0B0-2AB8-4D4E-BF49-3EE9470B1680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983312A7-07B0-804C-B101-08AF253AD641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27520" yWindow="2800" windowWidth="23120" windowHeight="23040" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
   <si>
     <t>Variables</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>2 promedios semestrales previos</t>
-  </si>
-  <si>
-    <t>2 promedios acumulados previos</t>
-  </si>
-  <si>
     <t>Hipotesis: ____</t>
   </si>
   <si>
@@ -107,9 +101,6 @@
     <t>La familia del estudiante tiene problemas financieros y esto le afecta</t>
   </si>
   <si>
-    <t>promedio heterogeneidad cursos</t>
-  </si>
-  <si>
     <t>resultados por areas ICFES</t>
   </si>
   <si>
@@ -131,18 +122,6 @@
     <t>Demografia estudiante:  edad en el semestre</t>
   </si>
   <si>
-    <t>Demografia estudiante:  genero</t>
-  </si>
-  <si>
-    <t>Demografia docente:  distribución por genero</t>
-  </si>
-  <si>
-    <t>promedio tamaño cursos que ha tomado ultimos 2 semestres</t>
-  </si>
-  <si>
-    <t>carga academica ultimos 2 semestres</t>
-  </si>
-  <si>
     <t>Carga creditos ultimos 2 semestres</t>
   </si>
   <si>
@@ -231,6 +210,33 @@
   </si>
   <si>
     <t>FECHA:  3 DE NOVIEMBRE</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>Promedio obtenidos semestres anteriores</t>
+  </si>
+  <si>
+    <t>Asignaturas vistas antes de tomar este semestre, indicandoel nivel de nota que sacó</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>promedio tamaño cursos tomados en el pasado</t>
+  </si>
+  <si>
+    <t>carga academica (cant cursos) ultimos 2 semestres</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
+  <si>
+    <t>3.12</t>
   </si>
 </sst>
 </file>
@@ -301,12 +307,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -321,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,7 +386,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -685,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
-  <dimension ref="A2:M94"/>
+  <dimension ref="A2:M89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,7 +729,7 @@
   <sheetData>
     <row r="2" spans="1:13" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -720,28 +741,28 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6"/>
@@ -750,28 +771,28 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9"/>
@@ -780,28 +801,28 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D12" s="9"/>
     </row>
@@ -811,35 +832,35 @@
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="C14" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="I14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="K14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="8" t="s">
+      <c r="L14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="M14" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -857,13 +878,13 @@
         <v>1</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>1</v>
@@ -883,13 +904,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
@@ -904,184 +925,182 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>3</v>
+        <v>22</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:13" ht="75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="4"/>
+      <c r="I20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>33</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="4"/>
+      <c r="J22" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>8</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>40</v>
+        <v>10</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K23" s="4"/>
       <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>9</v>
-      </c>
-      <c r="B24" s="11" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="D24" s="12"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
-      <c r="M24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="25" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
       <c r="B25" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>46</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D25" s="12"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>11</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>31</v>
-      </c>
+    <row r="26" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="12"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1091,12 +1110,13 @@
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>12</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>32</v>
+    <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="4"/>
@@ -1105,18 +1125,16 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
     <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="4"/>
@@ -1125,13 +1143,15 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>48</v>
@@ -1146,33 +1166,37 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
-    <row r="30" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>13</v>
+      </c>
       <c r="B30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="12"/>
+        <v>58</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="K30" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="L30" s="4"/>
     </row>
-    <row r="31" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
+    <row r="31" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>14</v>
+      </c>
       <c r="B31" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="12"/>
+        <v>62</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1180,37 +1204,44 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="8" t="s">
-        <v>52</v>
+      <c r="L31" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>16</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="12"/>
+        <v>64</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="4"/>
+      <c r="L32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:13" ht="68" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="16" t="s">
-        <v>54</v>
+      <c r="M32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>17</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="12"/>
+        <v>28</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1219,10 +1250,19 @@
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1230,18 +1270,10 @@
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
-      <c r="K34" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>14</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>33</v>
-      </c>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1249,16 +1281,14 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="L35" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>15</v>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B36" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1267,16 +1297,14 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>16</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>34</v>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B37" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1285,20 +1313,9 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M37" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>17</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1307,9 +1324,6 @@
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
-      <c r="M38" t="s">
-        <v>1</v>
-      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E39" s="4"/>
@@ -1321,7 +1335,13 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -1331,12 +1351,9 @@
       <c r="K40" s="4"/>
       <c r="L40" s="4"/>
     </row>
-    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="B41" s="8" t="s">
-        <v>56</v>
-      </c>
+    <row r="41" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="C41" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1347,12 +1364,9 @@
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
     </row>
-    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="B42" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>59</v>
+    <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="C42" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -1363,7 +1377,10 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="C43" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1383,13 +1400,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
     </row>
-    <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="B45" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>61</v>
-      </c>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -1399,10 +1410,7 @@
       <c r="K45" s="4"/>
       <c r="L45" s="4"/>
     </row>
-    <row r="46" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="C46" s="6" t="s">
-        <v>62</v>
-      </c>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1412,10 +1420,7 @@
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
     </row>
-    <row r="47" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="C47" s="6" t="s">
-        <v>63</v>
-      </c>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1425,10 +1430,7 @@
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
     </row>
-    <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="C48" s="6" t="s">
-        <v>64</v>
-      </c>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -1848,56 +1850,6 @@
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
     </row>
-    <row r="90" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E90" s="4"/>
-      <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
-      <c r="I90" s="4"/>
-      <c r="J90" s="4"/>
-      <c r="K90" s="4"/>
-      <c r="L90" s="4"/>
-    </row>
-    <row r="91" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="4"/>
-      <c r="K91" s="4"/>
-      <c r="L91" s="4"/>
-    </row>
-    <row r="92" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E92" s="4"/>
-      <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
-      <c r="K92" s="4"/>
-      <c r="L92" s="4"/>
-    </row>
-    <row r="93" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E93" s="4"/>
-      <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
-      <c r="J93" s="4"/>
-      <c r="K93" s="4"/>
-      <c r="L93" s="4"/>
-    </row>
-    <row r="94" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E94" s="4"/>
-      <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
-      <c r="I94" s="4"/>
-      <c r="J94" s="4"/>
-      <c r="K94" s="4"/>
-      <c r="L94" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:J2"/>

</xml_diff>

<commit_message>
ya se introdujeron dadtos de carga y creditos semestres anteriores..  y se hizo pruebas tanto con oversampling como downsampling..  y se calcula el ROC-AUC
</commit_message>
<xml_diff>
--- a/HIPOTESIS vs VARIABLES.xlsx
+++ b/HIPOTESIS vs VARIABLES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaimereinoso/DESARROLLO/UAOPiloto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983312A7-07B0-804C-B101-08AF253AD641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F36BD18-FEE2-944F-8E44-13F073202D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27520" yWindow="2800" windowWidth="23120" windowHeight="23040" xr2:uid="{39CEEB48-BA89-6646-9FA2-E7EBD1FB111A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>Variables</t>
   </si>
@@ -230,13 +230,19 @@
     <t>promedio tamaño cursos tomados en el pasado</t>
   </si>
   <si>
-    <t>carga academica (cant cursos) ultimos 2 semestres</t>
-  </si>
-  <si>
     <t>3.11</t>
   </si>
   <si>
     <t>3.12</t>
+  </si>
+  <si>
+    <t>carga academica (cant cursos) anteriores semestres</t>
+  </si>
+  <si>
+    <t>3.13</t>
+  </si>
+  <si>
+    <t>Cantidad de creditos perdidos en semestres anteriores</t>
   </si>
 </sst>
 </file>
@@ -316,13 +322,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,6 +393,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -706,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39A78E9-D45D-3D4E-A52F-2B0492CA372F}">
-  <dimension ref="A2:M89"/>
+  <dimension ref="A2:M90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1212,11 +1221,11 @@
       <c r="A32" s="1">
         <v>16</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>65</v>
+      <c r="B32" s="17" t="s">
+        <v>64</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -1236,8 +1245,8 @@
       <c r="A33" s="1">
         <v>17</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>66</v>
+      <c r="B33" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>28</v>
@@ -1254,15 +1263,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>18</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>61</v>
+      <c r="B34" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1273,7 +1282,16 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>19</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1283,13 +1301,7 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
     </row>
-    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>50</v>
-      </c>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1301,10 +1313,10 @@
     </row>
     <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -1315,7 +1327,13 @@
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B38" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1335,13 +1353,7 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
     </row>
-    <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="B40" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>54</v>
-      </c>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -1352,8 +1364,11 @@
       <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:13" ht="34" x14ac:dyDescent="0.2">
+      <c r="B41" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="C41" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1366,7 +1381,7 @@
     </row>
     <row r="42" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="C42" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -1377,9 +1392,9 @@
       <c r="K42" s="4"/>
       <c r="L42" s="4"/>
     </row>
-    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="C43" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -1390,7 +1405,10 @@
       <c r="K43" s="4"/>
       <c r="L43" s="4"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="C44" s="6" t="s">
+        <v>57</v>
+      </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -1850,6 +1868,16 @@
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
     </row>
+    <row r="90" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="4"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C2:J2"/>

</xml_diff>